<commit_message>
IEGC VIOLATION FORMATTING DONE
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -3,31 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D415540-AB91-460B-A82F-A47B138625F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436832D6-2AF3-4F56-B136-1A14760156DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>connStr</t>
+    <t>appDbConStr</t>
   </si>
   <si>
     <t>mis_warehouse/wrldc#123@10.2.100.56:15210/ORCLWR</t>
@@ -81,8 +71,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
@@ -424,47 +413,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="71.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{5FA4D75D-EC2C-488E-8936-58583A8ECC48}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>